<commit_message>
[JupyterEngineeringTemplate] Added implementation for GraphWriter.Updated Engineering Template Test.ipynb and Jupyter Engineering Template Requirements.xlsx
</commit_message>
<xml_diff>
--- a/python_source/EngineeringTemplate/files/Jupyter Engineering Template Requirements.xlsx
+++ b/python_source/EngineeringTemplate/files/Jupyter Engineering Template Requirements.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="REQUIREMENTS" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="86">
   <si>
     <t xml:space="preserve">Create library code for the jupyter notebook. (PTCC Module)</t>
   </si>
@@ -71,7 +71,7 @@
     <t xml:space="preserve">5. Can add headers or caption in the table</t>
   </si>
   <si>
-    <t xml:space="preserve">TASKS [JUPYTER ENGINEERING TEMPLATE]</t>
+    <t xml:space="preserve">JUPYTER ENGINEERING TEMPLATE</t>
   </si>
   <si>
     <t xml:space="preserve">Defining Equations</t>
@@ -230,49 +230,55 @@
     <t xml:space="preserve">Study Matplotlib</t>
   </si>
   <si>
+    <t xml:space="preserve">Adding multiple lines/functions/plot in the graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding title of the graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adding x and y axis labels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adding legends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on/off grids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">different plot/point types and color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multiple axes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 independent axs on the same axes</t>
+  </si>
+  <si>
     <t xml:space="preserve">ONGOING</t>
   </si>
   <si>
-    <t xml:space="preserve">Adding x and y values</t>
+    <t xml:space="preserve">Other tasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom Display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          ** create show method for all Writer Class.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          ** create toggle method for hiding cells in jupyter notebook.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          ** Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Writer Base Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Compare and Conclude Methods (From Warren's code)</t>
   </si>
   <si>
     <t xml:space="preserve">NOT STARTED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adding title of the graph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adding x and y axis labels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adding legends</t>
-  </si>
-  <si>
-    <t xml:space="preserve">on/off grids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">different plot types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other tasks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Custom Display</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          ** create show method for all Writer Class.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          ** create toggle method for hiding cells in jupyter notebook.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          ** Document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Writer Base Class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Compare and Conclude Methods (From Warren's code)</t>
   </si>
 </sst>
 </file>
@@ -287,6 +293,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -308,6 +315,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -359,7 +367,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -374,6 +382,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -395,14 +407,14 @@
   </sheetPr>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="61.87"/>
   </cols>
   <sheetData>
@@ -502,16 +514,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E60" activeCellId="0" sqref="E60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.56"/>
   </cols>
   <sheetData>
@@ -994,94 +1006,94 @@
         <v>68</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2"/>
       <c r="B60" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2"/>
       <c r="B61" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2"/>
       <c r="B63" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2"/>
       <c r="B64" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2"/>
       <c r="B65" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2"/>
+      <c r="B67" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B67" s="2"/>
-      <c r="C67" s="3" t="s">
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B69" s="2"/>
+      <c r="C69" s="3" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2"/>
       <c r="B70" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>20</v>
@@ -1090,7 +1102,7 @@
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2"/>
       <c r="B71" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>20</v>
@@ -1099,7 +1111,7 @@
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2"/>
       <c r="B72" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>20</v>
@@ -1108,22 +1120,40 @@
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2"/>
       <c r="B73" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>71</v>
+      <c r="C74" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C4:C31 C33:C41 C44:C48 C51:C56 C59:C65 C68:C73" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C4:C31 C33:C41 C44:C48 C51:C56 C59:C67 C70:C75" type="list">
       <formula1>"NOT STARTED,ONGOING,DONE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="86" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="86" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[JupyterEngineeringTemplate] updated task lists.
</commit_message>
<xml_diff>
--- a/python_source/EngineeringTemplate/files/Jupyter Engineering Template Requirements.xlsx
+++ b/python_source/EngineeringTemplate/files/Jupyter Engineering Template Requirements.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\PTCC_SCRIPTS\python_source\EngineeringTemplate\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="REQUIREMENTS" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="TASKS" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="REQUIREMENTS" sheetId="1" r:id="rId1"/>
+    <sheet name="TASKS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -21,81 +25,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="86">
-  <si>
-    <t xml:space="preserve">Create library code for the jupyter notebook. (PTCC Module)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Functional Requirements:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Engineers can define an equation with annotation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Engineers can create headers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. Engineers can define font style and font name for all their text.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. Engineers can add an image.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5. Engineers can create table and add their own data, cells can be merged.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6. Engineers can add graphs.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7. Engineers can export the jupyter notebook to pdf.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8. Engineers can add notes (should implement as add text).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-Functional Requirements:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Equation can be evaluated or not.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Can handle unit evaluation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. Can add headers or caption in the Image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. Can add information in a graph.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5. Can add headers or caption in the table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JUPYTER ENGINEERING TEMPLATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defining Equations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STATUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">converting expression in string to expression in latex (output to jupyter notebook)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DONE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">evaluating sympy expression. (results can be inline or next line)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rounding sympy expression from num_decimal user input</t>
-  </si>
-  <si>
-    <t xml:space="preserve">evaluating sympy expressions with units.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adding inline annotations.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="86">
+  <si>
+    <t>Create library code for the jupyter notebook. (PTCC Module)</t>
+  </si>
+  <si>
+    <t>Functional Requirements:</t>
+  </si>
+  <si>
+    <t>1. Engineers can define an equation with annotation.</t>
+  </si>
+  <si>
+    <t>2. Engineers can create headers</t>
+  </si>
+  <si>
+    <t>3. Engineers can define font style and font name for all their text.</t>
+  </si>
+  <si>
+    <t>4. Engineers can add an image.</t>
+  </si>
+  <si>
+    <t>5. Engineers can create table and add their own data, cells can be merged.</t>
+  </si>
+  <si>
+    <t>6. Engineers can add graphs.</t>
+  </si>
+  <si>
+    <t>7. Engineers can export the jupyter notebook to pdf.</t>
+  </si>
+  <si>
+    <t>8. Engineers can add notes (should implement as add text).</t>
+  </si>
+  <si>
+    <t>Non-Functional Requirements:</t>
+  </si>
+  <si>
+    <t>1. Equation can be evaluated or not.</t>
+  </si>
+  <si>
+    <t>2. Can handle unit evaluation.</t>
+  </si>
+  <si>
+    <t>3. Can add headers or caption in the Image</t>
+  </si>
+  <si>
+    <t>4. Can add information in a graph.</t>
+  </si>
+  <si>
+    <t>5. Can add headers or caption in the table</t>
+  </si>
+  <si>
+    <t>JUPYTER ENGINEERING TEMPLATE</t>
+  </si>
+  <si>
+    <t>Defining Equations</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>converting expression in string to expression in latex (output to jupyter notebook)</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>evaluating sympy expression. (results can be inline or next line)</t>
+  </si>
+  <si>
+    <t>rounding sympy expression from num_decimal user input</t>
+  </si>
+  <si>
+    <t>evaluating sympy expressions with units.</t>
+  </si>
+  <si>
+    <t>adding inline annotations.</t>
   </si>
   <si>
     <t xml:space="preserve">             ** Primary Annotation</t>
@@ -104,16 +108,16 @@
     <t xml:space="preserve">             ** Secondary Annotation</t>
   </si>
   <si>
-    <t xml:space="preserve">add implementation for adjusting font size and font name when defining equation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">appearance improvements</t>
+    <t>add implementation for adjusting font size and font name when defining equation</t>
+  </si>
+  <si>
+    <t>appearance improvements</t>
   </si>
   <si>
     <t xml:space="preserve">             ** horizontal and vertical spacings.</t>
   </si>
   <si>
-    <t xml:space="preserve">testing</t>
+    <t>testing</t>
   </si>
   <si>
     <t xml:space="preserve">              1. Fraction</t>
@@ -161,46 +165,46 @@
     <t xml:space="preserve">              11. very long equation</t>
   </si>
   <si>
-    <t xml:space="preserve">Document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defining Text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Define text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adding support for Font Styles (Italic, Bold, underline)</t>
+    <t>Document</t>
+  </si>
+  <si>
+    <t>Defining Text</t>
+  </si>
+  <si>
+    <t>Define text</t>
+  </si>
+  <si>
+    <t>Adding support for Font Styles (Italic, Bold, underline)</t>
   </si>
   <si>
     <t xml:space="preserve">              ** Add support for combinations of font styles</t>
   </si>
   <si>
-    <t xml:space="preserve">Adding support for Font Name (default is Arial)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adding support for Font Size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adding support for Text Position (CENTER, LEFT, RIGHT)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adding support for horizontal and vertical spaces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defining Image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add support for defining multiple images with captions.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">add support for horizontal and vertical layouting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">add support for width and height adjustment</t>
+    <t>Adding support for Font Name (default is Arial)</t>
+  </si>
+  <si>
+    <t>Adding support for Font Size</t>
+  </si>
+  <si>
+    <t>Adding support for Text Position (CENTER, LEFT, RIGHT)</t>
+  </si>
+  <si>
+    <t>Adding support for horizontal and vertical spaces</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Defining Image</t>
+  </si>
+  <si>
+    <t>Add support for defining multiple images with captions.</t>
+  </si>
+  <si>
+    <t>add support for horizontal and vertical layouting</t>
+  </si>
+  <si>
+    <t>add support for width and height adjustment</t>
   </si>
   <si>
     <t xml:space="preserve">Testing </t>
@@ -209,58 +213,55 @@
     <t xml:space="preserve">Document </t>
   </si>
   <si>
-    <t xml:space="preserve">Defining Table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">create table from list of string. -&gt; list of rows:string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add support for adding header of the table.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add support for adding table body</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Able to support spanning of rows and columns for each cell in the table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defining Graph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Study Matplotlib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adding multiple lines/functions/plot in the graph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adding title of the graph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adding x and y axis labels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adding legends</t>
-  </si>
-  <si>
-    <t xml:space="preserve">on/off grids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">different plot/point types and color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">multiple axes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 independent axs on the same axes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ONGOING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other tasks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Custom Display</t>
+    <t>Defining Table</t>
+  </si>
+  <si>
+    <t>create table from list of string. -&gt; list of rows:string</t>
+  </si>
+  <si>
+    <t>Add support for adding header of the table.</t>
+  </si>
+  <si>
+    <t>Add support for adding table body</t>
+  </si>
+  <si>
+    <t>Able to support spanning of rows and columns for each cell in the table</t>
+  </si>
+  <si>
+    <t>Defining Graph</t>
+  </si>
+  <si>
+    <t>Study Matplotlib</t>
+  </si>
+  <si>
+    <t>Adding multiple lines/functions/plot in the graph</t>
+  </si>
+  <si>
+    <t>Adding title of the graph</t>
+  </si>
+  <si>
+    <t>adding x and y axis labels</t>
+  </si>
+  <si>
+    <t>adding legends</t>
+  </si>
+  <si>
+    <t>on/off grids</t>
+  </si>
+  <si>
+    <t>different plot/point types and color</t>
+  </si>
+  <si>
+    <t>multiple axes</t>
+  </si>
+  <si>
+    <t>2 independent axs on the same axes</t>
+  </si>
+  <si>
+    <t>Other tasks</t>
+  </si>
+  <si>
+    <t>Custom Display</t>
   </si>
   <si>
     <t xml:space="preserve">          ** create show method for all Writer Class.</t>
@@ -272,23 +273,23 @@
     <t xml:space="preserve">          ** Document</t>
   </si>
   <si>
-    <t xml:space="preserve">Writer Base Class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create Compare and Conclude Methods (From Warren's code)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOT STARTED</t>
+    <t>Writer Base Class</t>
+  </si>
+  <si>
+    <t>Create Compare and Conclude Methods (From Warren's code)</t>
+  </si>
+  <si>
+    <t>NOT STARTED</t>
+  </si>
+  <si>
+    <t>Fix bug in simplifying equations with units.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -296,22 +297,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -326,183 +312,432 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+  <borders count="3">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="61.87"/>
+    <col min="1" max="1" width="49.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="61.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="0" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="0" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="0" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="0" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="0" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="0" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="0" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="0" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="0" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="0" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="0" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="0" t="s">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="0" t="s">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="86" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup scale="86" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -510,29 +745,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E60" activeCellId="0" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.56"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="66.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -541,7 +773,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>19</v>
@@ -550,7 +782,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>21</v>
@@ -559,7 +791,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>22</v>
@@ -568,7 +800,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -577,7 +809,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>24</v>
@@ -586,7 +818,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>25</v>
@@ -595,7 +827,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>26</v>
@@ -604,7 +836,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
         <v>27</v>
@@ -613,7 +845,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>28</v>
@@ -622,7 +854,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>29</v>
@@ -631,7 +863,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
         <v>30</v>
@@ -640,7 +872,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
         <v>31</v>
@@ -649,7 +881,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
         <v>32</v>
@@ -658,7 +890,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
         <v>33</v>
@@ -667,7 +899,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
         <v>34</v>
@@ -676,7 +908,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
         <v>35</v>
@@ -685,7 +917,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
         <v>36</v>
@@ -694,7 +926,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
         <v>37</v>
@@ -703,7 +935,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
         <v>38</v>
@@ -712,7 +944,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
         <v>39</v>
@@ -721,7 +953,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
         <v>40</v>
@@ -730,7 +962,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
         <v>41</v>
@@ -739,7 +971,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
         <v>42</v>
@@ -748,7 +980,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
         <v>43</v>
@@ -757,7 +989,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
         <v>44</v>
@@ -766,7 +998,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
         <v>45</v>
@@ -775,7 +1007,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
         <v>46</v>
@@ -784,7 +1016,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>47</v>
       </c>
@@ -793,7 +1025,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
         <v>48</v>
@@ -802,7 +1034,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
         <v>49</v>
@@ -811,7 +1043,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
         <v>50</v>
@@ -820,7 +1052,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
         <v>51</v>
@@ -829,7 +1061,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
         <v>52</v>
@@ -838,7 +1070,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
         <v>53</v>
@@ -847,7 +1079,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
         <v>54</v>
@@ -856,7 +1088,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
         <v>55</v>
@@ -865,7 +1097,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
         <v>46</v>
@@ -874,7 +1106,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>56</v>
       </c>
@@ -883,7 +1115,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
         <v>57</v>
@@ -892,7 +1124,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
         <v>58</v>
@@ -901,7 +1133,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
         <v>59</v>
@@ -910,7 +1142,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
         <v>60</v>
@@ -919,7 +1151,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
         <v>61</v>
@@ -928,7 +1160,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>62</v>
       </c>
@@ -937,7 +1169,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="2" t="s">
         <v>63</v>
@@ -946,7 +1178,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
         <v>64</v>
@@ -955,7 +1187,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
         <v>65</v>
@@ -964,7 +1196,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
         <v>66</v>
@@ -973,7 +1205,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2" t="s">
         <v>60</v>
@@ -982,7 +1214,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
         <v>61</v>
@@ -991,7 +1223,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>67</v>
       </c>
@@ -1000,7 +1232,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="2" t="s">
         <v>68</v>
@@ -1009,7 +1241,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="2" t="s">
         <v>69</v>
@@ -1018,7 +1250,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="2" t="s">
         <v>70</v>
@@ -1027,7 +1259,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
         <v>71</v>
@@ -1036,7 +1268,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="2" t="s">
         <v>72</v>
@@ -1045,7 +1277,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="2" t="s">
         <v>73</v>
@@ -1054,7 +1286,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="2" t="s">
         <v>74</v>
@@ -1063,7 +1295,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="2" t="s">
         <v>75</v>
@@ -1072,94 +1304,102 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C75" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="2"/>
+      <c r="B76" s="5" t="s">
         <v>85</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C4:C31 C33:C41 C44:C48 C51:C56 C59:C67 C70:C75" type="list">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C4:C31 C33:C41 C44:C48 C51:C56 C59:C67 C70:C76">
       <formula1>"NOT STARTED,ONGOING,DONE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="86" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup scale="86" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="41" man="true" max="16383" min="0"/>
+    <brk id="41" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>